<commit_message>
add experiment and results
</commit_message>
<xml_diff>
--- a/results/DRSA/FileDRSA_DOMLEM_NEW0.xlsx
+++ b/results/DRSA/FileDRSA_DOMLEM_NEW0.xlsx
@@ -407,7 +407,7 @@
     <t>Reguła 7</t>
   </si>
   <si>
-    <t>(attempts &gt;=  3.0) &amp; (pregnancy &lt;=  0.0) =&gt; (class &lt;= 1) ['a1', 'a7', 'a3']</t>
+    <t>(attempts &gt;=  3.0) &amp; (pregnancy &lt;=  0.0) =&gt; (class &lt;= 1) ['a1', 'a3', 'a7']</t>
   </si>
   <si>
     <t>(sperm &gt;=  3.0) =&gt; (class &lt;= 1) ['a25', 'a22']</t>
@@ -419,13 +419,13 @@
     <t>(attempts &gt;=  3.0) &amp; (sperm &gt;=  2.0) =&gt; (class &lt;= 1) ['a13']</t>
   </si>
   <si>
-    <t>(age &gt;=  42.0) =&gt; (class &lt;= 1) ['a14', 'a3']</t>
-  </si>
-  <si>
-    <t>(age &lt;=  31.0) &amp; (attempts &lt;=  1.0) &amp; (endometrium &lt;=  1.0) =&gt; (class &gt;= 2) ['a11', 'a9', 'a24', 'a12']</t>
-  </si>
-  <si>
-    <t>(frozen_embryos &gt;=  8.0) &amp; (sperm &lt;=  1.0) =&gt; (class &gt;= 2) ['a16', 'a6']</t>
+    <t>(age &gt;=  42.0) =&gt; (class &lt;= 1) ['a3', 'a14']</t>
+  </si>
+  <si>
+    <t>(age &lt;=  31.0) &amp; (attempts &lt;=  1.0) &amp; (endometrium &lt;=  1.0) =&gt; (class &gt;= 2) ['a11', 'a24', 'a12', 'a9']</t>
+  </si>
+  <si>
+    <t>(frozen_embryos &gt;=  8.0) &amp; (sperm &lt;=  1.0) =&gt; (class &gt;= 2) ['a6', 'a16']</t>
   </si>
   <si>
     <t>support</t>
@@ -437,16 +437,16 @@
     <t>coverage</t>
   </si>
   <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>not_classified</t>
+  </si>
+  <si>
+    <t>f1_score</t>
+  </si>
+  <si>
     <t>accuracy</t>
-  </si>
-  <si>
-    <t>not_classified</t>
-  </si>
-  <si>
-    <t>correct</t>
-  </si>
-  <si>
-    <t>f1_score</t>
   </si>
   <si>
     <t>Obiekt</t>
@@ -1666,7 +1666,7 @@
         <v>137</v>
       </c>
       <c r="B1">
-        <v>0.36</v>
+        <v>0.6923076923076923</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>139</v>
       </c>
       <c r="B3">
-        <v>0.6923076923076923</v>
+        <v>0.4466666666666665</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1690,7 +1690,7 @@
         <v>140</v>
       </c>
       <c r="B4">
-        <v>0.4466666666666665</v>
+        <v>0.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add correct results and results to debug of domapriori
</commit_message>
<xml_diff>
--- a/results/DRSA/FileDRSA_DOMLEM_NEW0.xlsx
+++ b/results/DRSA/FileDRSA_DOMLEM_NEW0.xlsx
@@ -407,25 +407,25 @@
     <t>Reguła 7</t>
   </si>
   <si>
-    <t>(attempts &gt;=  3.0) &amp; (pregnancy &lt;=  0.0) =&gt; (class &lt;= 1) ['a1', 'a3', 'a7']</t>
-  </si>
-  <si>
-    <t>(sperm &gt;=  3.0) =&gt; (class &lt;= 1) ['a25', 'a22']</t>
-  </si>
-  <si>
-    <t>(age &gt;=  40.0) &amp; (pregnancy &lt;=  0.0) =&gt; (class &lt;= 1) ['a15', 'a3']</t>
+    <t>(attempts &gt;=  3.0) &amp; (pregnancy &lt;=  0.0) =&gt; (class &lt;= 1) ['a3', 'a7', 'a1']</t>
+  </si>
+  <si>
+    <t>(sperm &gt;=  3.0) =&gt; (class &lt;= 1) ['a22', 'a25']</t>
+  </si>
+  <si>
+    <t>(age &gt;=  40.0) &amp; (pregnancy &lt;=  0.0) =&gt; (class &lt;= 1) ['a3', 'a15']</t>
   </si>
   <si>
     <t>(attempts &gt;=  3.0) &amp; (sperm &gt;=  2.0) =&gt; (class &lt;= 1) ['a13']</t>
   </si>
   <si>
-    <t>(age &gt;=  42.0) =&gt; (class &lt;= 1) ['a3', 'a14']</t>
-  </si>
-  <si>
-    <t>(age &lt;=  31.0) &amp; (attempts &lt;=  1.0) &amp; (endometrium &lt;=  1.0) =&gt; (class &gt;= 2) ['a11', 'a24', 'a12', 'a9']</t>
-  </si>
-  <si>
-    <t>(frozen_embryos &gt;=  8.0) &amp; (sperm &lt;=  1.0) =&gt; (class &gt;= 2) ['a6', 'a16']</t>
+    <t>(age &gt;=  42.0) =&gt; (class &lt;= 1) ['a14', 'a3']</t>
+  </si>
+  <si>
+    <t>(age &lt;=  31.0) &amp; (attempts &lt;=  1.0) &amp; (endometrium &lt;=  1.0) =&gt; (class &gt;= 2) ['a24', 'a9', 'a11', 'a12']</t>
+  </si>
+  <si>
+    <t>(frozen_embryos &gt;=  8.0) &amp; (sperm &lt;=  1.0) =&gt; (class &gt;= 2) ['a16', 'a6']</t>
   </si>
   <si>
     <t>support</t>
@@ -437,16 +437,16 @@
     <t>coverage</t>
   </si>
   <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>not_classified</t>
+  </si>
+  <si>
     <t>correct</t>
   </si>
   <si>
-    <t>not_classified</t>
-  </si>
-  <si>
     <t>f1_score</t>
-  </si>
-  <si>
-    <t>accuracy</t>
   </si>
   <si>
     <t>Obiekt</t>
@@ -1666,7 +1666,7 @@
         <v>137</v>
       </c>
       <c r="B1">
-        <v>0.6923076923076923</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>139</v>
       </c>
       <c r="B3">
-        <v>0.4466666666666665</v>
+        <v>0.6923076923076923</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1690,7 +1690,7 @@
         <v>140</v>
       </c>
       <c r="B4">
-        <v>0.36</v>
+        <v>0.4466666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -2789,7 +2789,7 @@
         <v>0.12</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2811,7 +2811,7 @@
         <v>0.08</v>
       </c>
       <c r="C4">
-        <v>0.3333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:3">

</xml_diff>